<commit_message>
prelude of chart for MOB
</commit_message>
<xml_diff>
--- a/output/reporthouronactivity.xlsx
+++ b/output/reporthouronactivity.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -492,31 +492,31 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C2" t="n">
-        <v>879</v>
+        <v>453.632</v>
       </c>
       <c r="D2" t="n">
-        <v>1180</v>
+        <v>1225.662</v>
       </c>
       <c r="E2" t="n">
-        <v>118</v>
+        <v>481</v>
       </c>
       <c r="F2" t="n">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="G2" t="n">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="H2" t="n">
-        <v>144</v>
+        <v>258</v>
       </c>
       <c r="I2" t="n">
-        <v>1011.4</v>
+        <v>2122.9</v>
       </c>
       <c r="J2" t="n">
-        <v>16.6699624283172</v>
+        <v>-42.2647322059447</v>
       </c>
     </row>
     <row r="3">
@@ -526,31 +526,31 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>50</v>
+        <v>131</v>
       </c>
       <c r="D3" t="n">
-        <v>54</v>
+        <v>138</v>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>157</v>
+        <v>288</v>
       </c>
       <c r="J3" t="n">
-        <v>-65.60509554140128</v>
+        <v>-52.08333333333333</v>
       </c>
     </row>
     <row r="4">
@@ -560,22 +560,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>200</v>
+        <v>464</v>
       </c>
       <c r="D4" t="n">
-        <v>215</v>
+        <v>492</v>
       </c>
       <c r="E4" t="n">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="F4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G4" t="n">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -584,7 +584,7 @@
         <v>81</v>
       </c>
       <c r="J4" t="n">
-        <v>165.4320987654321</v>
+        <v>507.4074074074074</v>
       </c>
     </row>
     <row r="5">
@@ -594,235 +594,269 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C5" t="n">
-        <v>812</v>
+        <v>767</v>
       </c>
       <c r="D5" t="n">
-        <v>988</v>
+        <v>1189</v>
       </c>
       <c r="E5" t="n">
-        <v>123</v>
+        <v>341</v>
       </c>
       <c r="F5" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G5" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H5" t="n">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="I5" t="n">
-        <v>1467</v>
+        <v>1529</v>
       </c>
       <c r="J5" t="n">
-        <v>-32.65167007498297</v>
+        <v>-22.23675604970569</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>MSK</t>
+          <t>MOB PRE</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>118</v>
+        <v>744</v>
       </c>
       <c r="D6" t="n">
-        <v>122</v>
+        <v>806</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>159</v>
+        <v>1134</v>
       </c>
       <c r="J6" t="n">
-        <v>-23.27044025157232</v>
+        <v>-28.92416225749559</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>NOT</t>
+          <t>MSK</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>82</v>
+        <v>275</v>
       </c>
       <c r="D7" t="n">
-        <v>93</v>
+        <v>299</v>
       </c>
       <c r="E7" t="n">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>134</v>
+        <v>321</v>
       </c>
       <c r="J7" t="n">
-        <v>-30.59701492537313</v>
+        <v>-6.853582554517135</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>TEC</t>
+          <t>NOT</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>241</v>
+        <v>82</v>
       </c>
       <c r="D8" t="n">
-        <v>247</v>
+        <v>93</v>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>646</v>
+        <v>134</v>
       </c>
       <c r="J8" t="n">
-        <v>-61.76470588235294</v>
+        <v>-30.59701492537313</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>TST</t>
+          <t>TEC</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" t="n">
+        <v>502</v>
+      </c>
+      <c r="D9" t="n">
+        <v>529</v>
+      </c>
+      <c r="E9" t="n">
         <v>22</v>
       </c>
-      <c r="D9" t="n">
-        <v>24</v>
-      </c>
-      <c r="E9" t="n">
-        <v>2</v>
-      </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>98</v>
+        <v>1307</v>
       </c>
       <c r="J9" t="n">
-        <v>-75.51020408163265</v>
+        <v>-59.5256312165264</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>VIP</t>
+          <t>TST</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>2</v>
+        <v>70</v>
       </c>
       <c r="D10" t="n">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="E10" t="n">
+        <v>25</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
         <v>1</v>
       </c>
-      <c r="F10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0</v>
-      </c>
       <c r="H10" t="n">
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>2</v>
+        <v>191</v>
       </c>
       <c r="J10" t="n">
-        <v>50</v>
+        <v>-50.26178010471204</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
+          <t>VIP</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>2</v>
+      </c>
+      <c r="D11" t="n">
+        <v>4</v>
+      </c>
+      <c r="E11" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>4</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
           <t>WLC</t>
         </is>
       </c>
-      <c r="B11" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" t="n">
-        <v>42</v>
-      </c>
-      <c r="D11" t="n">
-        <v>42</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" t="n">
-        <v>61</v>
-      </c>
-      <c r="J11" t="n">
-        <v>-31.14754098360656</v>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>81</v>
+      </c>
+      <c r="D12" t="n">
+        <v>87</v>
+      </c>
+      <c r="E12" t="n">
+        <v>6</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>130</v>
+      </c>
+      <c r="J12" t="n">
+        <v>-33.07692307692308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
prelude of chart for MOB p.2
</commit_message>
<xml_diff>
--- a/output/reporthouronactivity.xlsx
+++ b/output/reporthouronactivity.xlsx
@@ -513,10 +513,10 @@
         <v>258</v>
       </c>
       <c r="I2" t="n">
-        <v>2122.9</v>
+        <v>2342.6</v>
       </c>
       <c r="J2" t="n">
-        <v>-42.2647322059447</v>
+        <v>-47.67941603346708</v>
       </c>
     </row>
     <row r="3">
@@ -547,10 +547,10 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>288</v>
+        <v>317</v>
       </c>
       <c r="J3" t="n">
-        <v>-52.08333333333333</v>
+        <v>-56.46687697160884</v>
       </c>
     </row>
     <row r="4">
@@ -615,10 +615,10 @@
         <v>58</v>
       </c>
       <c r="I5" t="n">
-        <v>1529</v>
+        <v>1680</v>
       </c>
       <c r="J5" t="n">
-        <v>-22.23675604970569</v>
+        <v>-29.22619047619047</v>
       </c>
     </row>
     <row r="6">
@@ -649,10 +649,10 @@
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>1134</v>
+        <v>1224</v>
       </c>
       <c r="J6" t="n">
-        <v>-28.92416225749559</v>
+        <v>-34.15032679738562</v>
       </c>
     </row>
     <row r="7">
@@ -683,10 +683,10 @@
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>321</v>
+        <v>356</v>
       </c>
       <c r="J7" t="n">
-        <v>-6.853582554517135</v>
+        <v>-16.01123595505618</v>
       </c>
     </row>
     <row r="8">
@@ -751,10 +751,10 @@
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>1307</v>
+        <v>1454</v>
       </c>
       <c r="J9" t="n">
-        <v>-59.5256312165264</v>
+        <v>-63.61760660247593</v>
       </c>
     </row>
     <row r="10">
@@ -785,10 +785,10 @@
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>191</v>
+        <v>208</v>
       </c>
       <c r="J10" t="n">
-        <v>-50.26178010471204</v>
+        <v>-54.32692307692308</v>
       </c>
     </row>
     <row r="11">
@@ -853,10 +853,10 @@
         <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>130</v>
+        <v>149</v>
       </c>
       <c r="J12" t="n">
-        <v>-33.07692307692308</v>
+        <v>-41.61073825503355</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refreshing chart with a timeframe using schedule
</commit_message>
<xml_diff>
--- a/output/reporthouronactivity.xlsx
+++ b/output/reporthouronactivity.xlsx
@@ -492,31 +492,31 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C2" t="n">
-        <v>889</v>
+        <v>764.322</v>
       </c>
       <c r="D2" t="n">
-        <v>1009</v>
+        <v>1112.327</v>
       </c>
       <c r="E2" t="n">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="F2" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="G2" t="n">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="H2" t="n">
-        <v>107</v>
+        <v>262</v>
       </c>
       <c r="I2" t="n">
-        <v>1008.8</v>
+        <v>2419.3</v>
       </c>
       <c r="J2" t="n">
-        <v>0.01982553528945274</v>
+        <v>-54.02277518290415</v>
       </c>
     </row>
     <row r="3">
@@ -529,28 +529,28 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="D3" t="n">
-        <v>83</v>
+        <v>192</v>
       </c>
       <c r="E3" t="n">
+        <v>12</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
         <v>5</v>
       </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="n">
-        <v>1</v>
-      </c>
       <c r="H3" t="n">
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>120</v>
+        <v>289</v>
       </c>
       <c r="J3" t="n">
-        <v>-30.83333333333334</v>
+        <v>-33.56401384083046</v>
       </c>
     </row>
     <row r="4">
@@ -563,19 +563,19 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>256</v>
+        <v>540</v>
       </c>
       <c r="D4" t="n">
-        <v>271</v>
+        <v>565</v>
       </c>
       <c r="E4" t="n">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="F4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G4" t="n">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -584,7 +584,7 @@
         <v>112</v>
       </c>
       <c r="J4" t="n">
-        <v>141.9642857142857</v>
+        <v>404.4642857142857</v>
       </c>
     </row>
     <row r="5">
@@ -594,31 +594,31 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>505</v>
+        <v>1041</v>
       </c>
       <c r="D5" t="n">
-        <v>547</v>
+        <v>1186</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G5" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="H5" t="n">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="I5" t="n">
-        <v>678</v>
+        <v>1469</v>
       </c>
       <c r="J5" t="n">
-        <v>-19.32153392330384</v>
+        <v>-19.2648059904697</v>
       </c>
     </row>
     <row r="6">
@@ -628,31 +628,31 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>498</v>
+        <v>930</v>
       </c>
       <c r="D6" t="n">
-        <v>519</v>
+        <v>976</v>
       </c>
       <c r="E6" t="n">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="F6" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G6" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>536</v>
+        <v>1148</v>
       </c>
       <c r="J6" t="n">
-        <v>-3.171641791044777</v>
+        <v>-14.98257839721254</v>
       </c>
     </row>
     <row r="7">
@@ -665,13 +665,13 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>130</v>
+        <v>260</v>
       </c>
       <c r="D7" t="n">
-        <v>132</v>
+        <v>266</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -683,10 +683,10 @@
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>165</v>
+        <v>390</v>
       </c>
       <c r="J7" t="n">
-        <v>-20</v>
+        <v>-31.79487179487179</v>
       </c>
     </row>
     <row r="8">
@@ -733,28 +733,28 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>219</v>
+        <v>425</v>
       </c>
       <c r="D9" t="n">
-        <v>222</v>
+        <v>430</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
         <v>2</v>
       </c>
       <c r="G9" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" t="n">
-        <v>591</v>
+        <v>1339</v>
       </c>
       <c r="J9" t="n">
-        <v>-62.43654822335025</v>
+        <v>-67.88648244958925</v>
       </c>
     </row>
     <row r="10">
@@ -767,28 +767,28 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>52</v>
+        <v>93</v>
       </c>
       <c r="D10" t="n">
-        <v>51</v>
+        <v>94</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>86</v>
+        <v>202</v>
       </c>
       <c r="J10" t="n">
-        <v>-40.69767441860465</v>
+        <v>-53.46534653465347</v>
       </c>
     </row>
     <row r="11">
@@ -819,10 +819,10 @@
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J11" t="n">
-        <v>33.33333333333333</v>
+        <v>-33.33333333333334</v>
       </c>
     </row>
     <row r="12">
@@ -835,28 +835,28 @@
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="D12" t="n">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="E12" t="n">
+        <v>2</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
         <v>1</v>
       </c>
-      <c r="F12" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0</v>
-      </c>
       <c r="H12" t="n">
         <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>68</v>
+        <v>157</v>
       </c>
       <c r="J12" t="n">
-        <v>-70.58823529411764</v>
+        <v>-66.87898089171975</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TO be Managed for SettingWithCopy -  not refreshing values on chart
</commit_message>
<xml_diff>
--- a/output/reporthouronactivity.xlsx
+++ b/output/reporthouronactivity.xlsx
@@ -492,31 +492,31 @@
         </is>
       </c>
       <c r="B2" t="n">
+        <v>13</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1400</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1504</v>
+      </c>
+      <c r="E2" t="n">
+        <v>17</v>
+      </c>
+      <c r="F2" t="n">
         <v>4</v>
       </c>
-      <c r="C2" t="n">
-        <v>606</v>
-      </c>
-      <c r="D2" t="n">
-        <v>634</v>
-      </c>
-      <c r="E2" t="n">
-        <v>7</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
-      </c>
       <c r="G2" t="n">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="H2" t="n">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="I2" t="n">
-        <v>707.2</v>
+        <v>1501.5</v>
       </c>
       <c r="J2" t="n">
-        <v>-10.35067873303168</v>
+        <v>0.166500166500172</v>
       </c>
     </row>
     <row r="3">
@@ -526,19 +526,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>59</v>
+        <v>136</v>
       </c>
       <c r="D3" t="n">
-        <v>62</v>
+        <v>145</v>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
         <v>2</v>
@@ -547,10 +547,10 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>81</v>
+        <v>148</v>
       </c>
       <c r="J3" t="n">
-        <v>-23.45679012345679</v>
+        <v>-2.027027027027029</v>
       </c>
     </row>
     <row r="4">
@@ -560,22 +560,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>161</v>
+        <v>327</v>
       </c>
       <c r="D4" t="n">
-        <v>172</v>
+        <v>351</v>
       </c>
       <c r="E4" t="n">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="F4" t="n">
         <v>2</v>
       </c>
       <c r="G4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -584,7 +584,7 @@
         <v>120</v>
       </c>
       <c r="J4" t="n">
-        <v>43.33333333333334</v>
+        <v>192.5</v>
       </c>
     </row>
     <row r="5">
@@ -597,28 +597,28 @@
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>390</v>
+        <v>789</v>
       </c>
       <c r="D5" t="n">
-        <v>404</v>
+        <v>829</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G5" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="H5" t="n">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="I5" t="n">
-        <v>504</v>
+        <v>926</v>
       </c>
       <c r="J5" t="n">
-        <v>-19.84126984126984</v>
+        <v>-10.47516198704104</v>
       </c>
     </row>
     <row r="6">
@@ -628,31 +628,31 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C6" t="n">
-        <v>277</v>
+        <v>627</v>
       </c>
       <c r="D6" t="n">
-        <v>333</v>
+        <v>707</v>
       </c>
       <c r="E6" t="n">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="F6" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G6" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" t="n">
-        <v>364</v>
+        <v>642</v>
       </c>
       <c r="J6" t="n">
-        <v>-8.51648351648352</v>
+        <v>10.12461059190031</v>
       </c>
     </row>
     <row r="7">
@@ -662,16 +662,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>100</v>
+        <v>186</v>
       </c>
       <c r="D7" t="n">
-        <v>101</v>
+        <v>190</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -683,10 +683,10 @@
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>110</v>
+        <v>196</v>
       </c>
       <c r="J7" t="n">
-        <v>-8.18181818181818</v>
+        <v>-3.061224489795922</v>
       </c>
     </row>
     <row r="8">
@@ -733,10 +733,10 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>185</v>
+        <v>364</v>
       </c>
       <c r="D9" t="n">
-        <v>185</v>
+        <v>364</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -745,16 +745,16 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>441</v>
+        <v>788</v>
       </c>
       <c r="J9" t="n">
-        <v>-58.0498866213152</v>
+        <v>-53.80710659898477</v>
       </c>
     </row>
     <row r="10">
@@ -764,13 +764,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C10" t="n">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="D10" t="n">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -785,10 +785,10 @@
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="J10" t="n">
-        <v>-24</v>
+        <v>-15.78947368421053</v>
       </c>
     </row>
     <row r="11">
@@ -801,10 +801,10 @@
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -819,10 +819,10 @@
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J11" t="n">
-        <v>-50</v>
+        <v>-25</v>
       </c>
     </row>
     <row r="12">
@@ -832,13 +832,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="D12" t="n">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -847,16 +847,16 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="J12" t="n">
-        <v>-43.18181818181818</v>
+        <v>-43.52941176470588</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
saving 10 min frame report
</commit_message>
<xml_diff>
--- a/output/reporthouronactivity.xlsx
+++ b/output/reporthouronactivity.xlsx
@@ -492,31 +492,31 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C2" t="n">
-        <v>339</v>
+        <v>1222</v>
       </c>
       <c r="D2" t="n">
-        <v>401</v>
+        <v>1499</v>
       </c>
       <c r="E2" t="n">
-        <v>12</v>
+        <v>106</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G2" t="n">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="H2" t="n">
-        <v>35</v>
+        <v>159</v>
       </c>
       <c r="I2" t="n">
-        <v>601.9</v>
+        <v>1595.1</v>
       </c>
       <c r="J2" t="n">
-        <v>-33.37763748130919</v>
+        <v>-6.024700645727532</v>
       </c>
     </row>
     <row r="3">
@@ -529,28 +529,28 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>46</v>
+        <v>163</v>
       </c>
       <c r="D3" t="n">
-        <v>49</v>
+        <v>165</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>79</v>
+        <v>158</v>
       </c>
       <c r="J3" t="n">
-        <v>-37.9746835443038</v>
+        <v>4.430379746835444</v>
       </c>
     </row>
     <row r="4">
@@ -560,22 +560,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>125</v>
+        <v>342</v>
       </c>
       <c r="D4" t="n">
-        <v>130</v>
+        <v>353</v>
       </c>
       <c r="E4" t="n">
+        <v>10</v>
+      </c>
+      <c r="F4" t="n">
         <v>3</v>
       </c>
-      <c r="F4" t="n">
-        <v>1</v>
-      </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -584,7 +584,7 @@
         <v>100</v>
       </c>
       <c r="J4" t="n">
-        <v>30</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5">
@@ -594,31 +594,31 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>281</v>
+        <v>875</v>
       </c>
       <c r="D5" t="n">
-        <v>311</v>
+        <v>1012</v>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="F5" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G5" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="H5" t="n">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="I5" t="n">
-        <v>558</v>
+        <v>1028</v>
       </c>
       <c r="J5" t="n">
-        <v>-44.2652329749104</v>
+        <v>-1.556420233463029</v>
       </c>
     </row>
     <row r="6">
@@ -628,31 +628,31 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C6" t="n">
-        <v>212</v>
+        <v>711</v>
       </c>
       <c r="D6" t="n">
-        <v>290</v>
+        <v>854</v>
       </c>
       <c r="E6" t="n">
-        <v>45</v>
+        <v>136</v>
       </c>
       <c r="F6" t="n">
+        <v>7</v>
+      </c>
+      <c r="G6" t="n">
         <v>4</v>
       </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
       <c r="H6" t="n">
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>366</v>
+        <v>758</v>
       </c>
       <c r="J6" t="n">
-        <v>-20.76502732240437</v>
+        <v>12.66490765171504</v>
       </c>
     </row>
     <row r="7">
@@ -665,28 +665,28 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>77</v>
+        <v>212</v>
       </c>
       <c r="D7" t="n">
-        <v>81</v>
+        <v>237</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>115</v>
+        <v>232</v>
       </c>
       <c r="J7" t="n">
-        <v>-29.56521739130434</v>
+        <v>2.155172413793105</v>
       </c>
     </row>
     <row r="8">
@@ -730,31 +730,31 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>131</v>
+        <v>302</v>
       </c>
       <c r="D9" t="n">
-        <v>131</v>
+        <v>305</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>392</v>
+        <v>821</v>
       </c>
       <c r="J9" t="n">
-        <v>-66.58163265306123</v>
+        <v>-62.85018270401949</v>
       </c>
     </row>
     <row r="10">
@@ -767,16 +767,16 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="D10" t="n">
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" t="n">
         <v>1</v>
@@ -785,10 +785,10 @@
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>47</v>
+        <v>107</v>
       </c>
       <c r="J10" t="n">
-        <v>-61.70212765957447</v>
+        <v>-25.23364485981309</v>
       </c>
     </row>
     <row r="11">
@@ -801,13 +801,13 @@
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -819,10 +819,10 @@
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J11" t="n">
-        <v>-100</v>
+        <v>-40</v>
       </c>
     </row>
     <row r="12">
@@ -835,13 +835,13 @@
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="D12" t="n">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -853,10 +853,10 @@
         <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>34</v>
+        <v>74</v>
       </c>
       <c r="J12" t="n">
-        <v>-61.76470588235294</v>
+        <v>-50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some details more to align chart starting from 8 for real-time line
</commit_message>
<xml_diff>
--- a/output/reporthouronactivity.xlsx
+++ b/output/reporthouronactivity.xlsx
@@ -492,13 +492,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>459.123</v>
+        <v>516.237</v>
       </c>
       <c r="D2" t="n">
-        <v>674.1279999999999</v>
+        <v>735.242</v>
       </c>
       <c r="E2" t="n">
         <v>77</v>
@@ -507,16 +507,16 @@
         <v>8</v>
       </c>
       <c r="G2" t="n">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="H2" t="n">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="I2" t="n">
-        <v>2139</v>
+        <v>2432</v>
       </c>
       <c r="J2" t="n">
-        <v>-68.48396446937821</v>
+        <v>-69.76800986842106</v>
       </c>
     </row>
     <row r="3">
@@ -529,10 +529,10 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="D3" t="n">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="E3" t="n">
         <v>2</v>
@@ -547,10 +547,10 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>181</v>
+        <v>216</v>
       </c>
       <c r="J3" t="n">
-        <v>-14.9171270718232</v>
+        <v>-22.22222222222222</v>
       </c>
     </row>
     <row r="4">
@@ -563,10 +563,10 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>279</v>
+        <v>290</v>
       </c>
       <c r="D4" t="n">
-        <v>285</v>
+        <v>296</v>
       </c>
       <c r="E4" t="n">
         <v>11</v>
@@ -575,16 +575,16 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>461</v>
+        <v>510</v>
       </c>
       <c r="J4" t="n">
-        <v>-38.17787418655097</v>
+        <v>-41.96078431372548</v>
       </c>
     </row>
     <row r="5">
@@ -597,10 +597,10 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>814</v>
+        <v>904</v>
       </c>
       <c r="D5" t="n">
-        <v>934</v>
+        <v>1026</v>
       </c>
       <c r="E5" t="n">
         <v>43</v>
@@ -609,16 +609,16 @@
         <v>6</v>
       </c>
       <c r="G5" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H5" t="n">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I5" t="n">
-        <v>1302</v>
+        <v>1434</v>
       </c>
       <c r="J5" t="n">
-        <v>-28.2642089093702</v>
+        <v>-28.45188284518828</v>
       </c>
     </row>
     <row r="6">
@@ -631,13 +631,13 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>469</v>
+        <v>510</v>
       </c>
       <c r="D6" t="n">
-        <v>510</v>
+        <v>554</v>
       </c>
       <c r="E6" t="n">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F6" t="n">
         <v>3</v>
@@ -649,10 +649,10 @@
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>1109</v>
+        <v>1232</v>
       </c>
       <c r="J6" t="n">
-        <v>-54.01262398557258</v>
+        <v>-55.03246753246754</v>
       </c>
     </row>
     <row r="7">
@@ -665,10 +665,10 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>227</v>
+        <v>256</v>
       </c>
       <c r="D7" t="n">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="E7" t="n">
         <v>30</v>
@@ -683,10 +683,10 @@
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>289</v>
+        <v>324</v>
       </c>
       <c r="J7" t="n">
-        <v>-11.07266435986159</v>
+        <v>-11.72839506172839</v>
       </c>
     </row>
     <row r="8">
@@ -699,10 +699,10 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>402</v>
+        <v>437</v>
       </c>
       <c r="D8" t="n">
-        <v>406</v>
+        <v>441</v>
       </c>
       <c r="E8" t="n">
         <v>3</v>
@@ -717,10 +717,10 @@
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>905</v>
+        <v>1013</v>
       </c>
       <c r="J8" t="n">
-        <v>-55.13812154696133</v>
+        <v>-56.4659427443238</v>
       </c>
     </row>
     <row r="9">
@@ -733,10 +733,10 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="D9" t="n">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="E9" t="n">
         <v>10</v>
@@ -745,16 +745,16 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>141</v>
+        <v>164</v>
       </c>
       <c r="J9" t="n">
-        <v>1.418439716312059</v>
+        <v>-4.878048780487809</v>
       </c>
     </row>
     <row r="10">
@@ -767,10 +767,10 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D10" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E10" t="n">
         <v>3</v>
@@ -788,7 +788,7 @@
         <v>4</v>
       </c>
       <c r="J10" t="n">
-        <v>75</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11">
@@ -801,10 +801,10 @@
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D11" t="n">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E11" t="n">
         <v>1</v>
@@ -813,16 +813,16 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="J11" t="n">
-        <v>-66.66666666666667</v>
+        <v>-67.56756756756756</v>
       </c>
     </row>
   </sheetData>

</xml_diff>